<commit_message>
hasta calculo de limiter
</commit_message>
<xml_diff>
--- a/componentes.xlsx
+++ b/componentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\mi_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8424EE05-306B-477D-8406-6168505FF225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93B5D98-52B1-402E-B586-0B4099F815E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$H$55</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -389,7 +389,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +400,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF5F5F5"/>
         <bgColor rgb="FFF5F5F5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFF5F5F5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -430,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -438,6 +450,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,8 +740,8 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,29 +879,29 @@
         <v>2652</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
         <v>49295.23</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="3">
         <v>33598</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="F6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3">
         <v>13627.38</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="3">
         <v>9213</v>
       </c>
     </row>
@@ -1253,29 +1269,29 @@
         <v>5782</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="3">
         <v>68590.58</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="3">
         <v>27531</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="1">
+      <c r="F21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="3">
         <v>5048.5020000000004</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="3">
         <v>2565</v>
       </c>
     </row>
@@ -1877,29 +1893,29 @@
         <v>791</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="3">
         <v>50051.43</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="3">
         <v>22514</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="1">
+      <c r="F45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="3">
         <v>14379.43</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H45" s="3">
         <v>8420</v>
       </c>
     </row>

</xml_diff>

<commit_message>
limiter y fecha estimada ajustado para empezar css
</commit_message>
<xml_diff>
--- a/componentes.xlsx
+++ b/componentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\mi_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93B5D98-52B1-402E-B586-0B4099F815E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F41098-D101-4B2D-A741-F2CFE79E23C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -389,7 +389,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +412,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFF5F5F5"/>
       </patternFill>
     </fill>
   </fills>
@@ -442,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -454,6 +460,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,7 +750,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +788,7 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -805,7 +814,7 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -831,7 +840,7 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -857,7 +866,7 @@
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -909,7 +918,7 @@
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -935,7 +944,7 @@
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1403,7 +1412,7 @@
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1429,7 +1438,7 @@
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1481,7 +1490,7 @@
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1507,7 +1516,7 @@
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1533,7 +1542,7 @@
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1741,7 +1750,7 @@
       <c r="A39" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1767,7 +1776,7 @@
       <c r="A40" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="5" t="s">
         <v>84</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1793,7 +1802,7 @@
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1923,7 +1932,7 @@
       <c r="A46" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1949,7 +1958,7 @@
       <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C47" s="1" t="s">

</xml_diff>